<commit_message>
update xlsx fine tuned
</commit_message>
<xml_diff>
--- a/2_fine_tuned/Reports/config_FT_vistas_121124.xlsx
+++ b/2_fine_tuned/Reports/config_FT_vistas_121124.xlsx
@@ -716,7 +716,7 @@
       </c>
       <c r="H2" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/EQUATORIAL_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/EQUATORIAL_R</t>
         </is>
       </c>
       <c r="I2" s="4" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="H3" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/POLAR_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/POLAR_R</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="H4" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/EQUATORIAL_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/EQUATORIAL_R</t>
         </is>
       </c>
       <c r="I4" s="4" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="H5" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/POLAR_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/POLAR_R</t>
         </is>
       </c>
       <c r="I5" s="4" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="H6" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/EQUATORIAL_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/EQUATORIAL_R</t>
         </is>
       </c>
       <c r="I6" s="4" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="H7" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/POLAR_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/POLAR_R</t>
         </is>
       </c>
       <c r="I7" s="4" t="inlineStr">
@@ -962,7 +962,7 @@
       </c>
       <c r="H8" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/EQUATORIAL_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/EQUATORIAL_R</t>
         </is>
       </c>
       <c r="I8" s="4" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="H9" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/POLAR_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/POLAR_R</t>
         </is>
       </c>
       <c r="I9" s="4" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="H10" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/EQUATORIAL_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/EQUATORIAL_R</t>
         </is>
       </c>
       <c r="I10" s="4" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="H11" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/POLAR_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/POLAR_R</t>
         </is>
       </c>
       <c r="I11" s="4" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="H12" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/EQUATORIAL_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/EQUATORIAL_R</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="H13" s="4" t="inlineStr">
         <is>
-          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_111124/POLAR_R</t>
+          <t>/media/jczars/4C22F02A22F01B22/Pollen_classification_view/BD/CPD1_Dn_VTcr_151124/POLAR_R</t>
         </is>
       </c>
       <c r="I13" s="4" t="inlineStr">
@@ -4125,7 +4125,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H4:H13 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="5">
       <c r="A1" s="4" t="inlineStr">

</xml_diff>